<commit_message>
Results file fix for 6144 sized GEMM kernels.
</commit_message>
<xml_diff>
--- a/results/inference/server/DeepBench_NV_1080Ti.xlsx
+++ b/results/inference/server/DeepBench_NV_1080Ti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37320" windowHeight="20640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results - Mixed Precision" sheetId="2" r:id="rId1"/>
@@ -1364,11 +1364,11 @@
         <v>2</v>
       </c>
       <c r="I26" s="3">
-        <v>1.1850000000000001</v>
+        <v>1.2170000000000001</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" si="0"/>
-        <v>31.855473417721516</v>
+        <v>31.017860312243222</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1510,11 +1510,11 @@
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="3">
-        <v>2.3050000000000002</v>
+        <v>2.266</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" si="0"/>
-        <v>32.753783947939255</v>
+        <v>33.317507502206524</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -1656,11 +1656,11 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="3">
-        <v>4.5030000000000001</v>
+        <v>4.0179999999999998</v>
       </c>
       <c r="J36" s="3">
         <f t="shared" si="0"/>
-        <v>33.532077281812128</v>
+        <v>37.579627675460429</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -1776,11 +1776,11 @@
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="3">
-        <v>5.0999999999999997E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="J40" s="3">
         <f t="shared" si="0"/>
-        <v>0.49344752941176473</v>
+        <v>0.57195054545454538</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -1866,11 +1866,11 @@
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="3">
-        <v>5.1999999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J43" s="3">
         <f t="shared" si="0"/>
-        <v>0.96791630769230774</v>
+        <v>1.2582911999999999</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -1956,11 +1956,11 @@
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="3">
-        <v>7.1999999999999995E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="J46" s="3">
         <f t="shared" si="0"/>
-        <v>1.3981013333333334</v>
+        <v>1.7061575593220339</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -9073,7 +9073,7 @@
         <v>28</v>
       </c>
       <c r="Q207" s="3">
-        <f t="shared" ref="Q207:Q238" si="14">(2*O207*P207*E207*F207*G207*I207*H207)/(N207/1000)/10^12</f>
+        <f t="shared" ref="Q207:Q217" si="14">(2*O207*P207*E207*F207*G207*I207*H207)/(N207/1000)/10^12</f>
         <v>10.816889263157895</v>
       </c>
       <c r="R207">

</xml_diff>